<commit_message>
add teleport after finish normal level
</commit_message>
<xml_diff>
--- a/Assets/_Excel/scene.xlsx
+++ b/Assets/_Excel/scene.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProject\Card\Card-game_test\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C573830-A34E-4B57-9732-2BB0D588B649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF74FC87-F669-422B-AB04-26C43C06DD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="3460" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3460" yWindow="4110" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
   <si>
     <t>Id</t>
   </si>
@@ -51,10 +51,34 @@
     <t>Battle Map Scene</t>
   </si>
   <si>
-    <t>UI/Ice2Prefab</t>
-  </si>
-  <si>
-    <t>UI/Ice3Prefab</t>
+    <t>Ice2Prefab</t>
+  </si>
+  <si>
+    <t>NormalEnemyAmount</t>
+  </si>
+  <si>
+    <t>BossEnemyAmount</t>
+  </si>
+  <si>
+    <t>Number of enemy</t>
+  </si>
+  <si>
+    <t>SpawnOne</t>
+  </si>
+  <si>
+    <t>SpawnTwo</t>
+  </si>
+  <si>
+    <t>SpawnThree</t>
+  </si>
+  <si>
+    <t>Spawn Enemy</t>
+  </si>
+  <si>
+    <t>Model/cheche(main)</t>
+  </si>
+  <si>
+    <t>Image/UI/Ice3</t>
   </si>
 </sst>
 </file>
@@ -372,15 +396,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,8 +417,23 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -407,8 +446,23 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -419,10 +473,25 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -433,10 +502,25 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -447,7 +531,22 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
able to add card and transition to next map main
</commit_message>
<xml_diff>
--- a/Assets/_Excel/scene.xlsx
+++ b/Assets/_Excel/scene.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Cards\Card-game-demo\Assets\_Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProject\Card\Card-game_test\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369A855F-B42A-41B9-8EB7-74AAA0394C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F8BAD5-CEF3-49B0-ABD9-57068EA67AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="1560" windowWidth="27525" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="3810" windowWidth="18850" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t>Id</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Model/Boss1_main</t>
+  </si>
+  <si>
+    <t>Image/UI/OceanMain</t>
   </si>
 </sst>
 </file>
@@ -133,7 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,12 +417,12 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,7 +457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -489,7 +492,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -524,12 +527,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1002</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -559,7 +562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1003</v>
       </c>

</xml_diff>